<commit_message>
Estilizacao das planilhas para facilitar o usuario
</commit_message>
<xml_diff>
--- a/dados/Resultado.xlsx
+++ b/dados/Resultado.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vini-\Documents\projetos\calculadora-viagem\dados\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E063E40-BFE1-4CF8-B144-9257F3A8E1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="resultado" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -25,9 +31,6 @@
     <t>Fernando</t>
   </si>
   <si>
-    <t>Felps</t>
-  </si>
-  <si>
     <t>Igor</t>
   </si>
   <si>
@@ -50,13 +53,16 @@
   </si>
   <si>
     <t>Vinicius</t>
+  </si>
+  <si>
+    <t>Felipe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,12 +71,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -85,21 +103,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -137,7 +165,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -171,6 +199,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -205,9 +234,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -380,53 +410,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -463,8 +498,8 @@
         <v>17.07</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -501,9 +536,9 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
-      <c r="A4" t="s">
-        <v>3</v>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B4">
         <v>23.36</v>
@@ -530,7 +565,7 @@
         <v>23.36</v>
       </c>
       <c r="J4">
-        <v>73.01000000000001</v>
+        <v>73.010000000000005</v>
       </c>
       <c r="K4">
         <v>23.36</v>
@@ -539,9 +574,9 @@
         <v>23.36</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s">
-        <v>4</v>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B5">
         <v>2.35</v>
@@ -577,9 +612,9 @@
         <v>9.57</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
-      <c r="A6" t="s">
-        <v>5</v>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B6">
         <v>16.79</v>
@@ -615,9 +650,9 @@
         <v>16.79</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
-      <c r="A7" t="s">
-        <v>6</v>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B7">
         <v>11.98</v>
@@ -653,47 +688,47 @@
         <v>11.98</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
-      <c r="A8" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" t="s">
-        <v>8</v>
       </c>
       <c r="B9">
         <v>19.52</v>
@@ -729,47 +764,47 @@
         <v>18.12</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
-      <c r="A10" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>3.48</v>
+      </c>
+      <c r="C10">
+        <v>3.48</v>
+      </c>
+      <c r="D10">
+        <v>3.48</v>
+      </c>
+      <c r="E10">
+        <v>3.48</v>
+      </c>
+      <c r="F10">
+        <v>3.48</v>
+      </c>
+      <c r="G10">
+        <v>3.48</v>
+      </c>
+      <c r="H10">
+        <v>3.48</v>
+      </c>
+      <c r="I10">
+        <v>3.48</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>3.48</v>
+      </c>
+      <c r="L10">
+        <v>3.48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B10">
-        <v>3.48</v>
-      </c>
-      <c r="C10">
-        <v>3.48</v>
-      </c>
-      <c r="D10">
-        <v>3.48</v>
-      </c>
-      <c r="E10">
-        <v>3.48</v>
-      </c>
-      <c r="F10">
-        <v>3.48</v>
-      </c>
-      <c r="G10">
-        <v>3.48</v>
-      </c>
-      <c r="H10">
-        <v>3.48</v>
-      </c>
-      <c r="I10">
-        <v>3.48</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>3.48</v>
-      </c>
-      <c r="L10">
-        <v>3.48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" t="s">
-        <v>10</v>
       </c>
       <c r="B11">
         <v>0.73</v>
@@ -805,9 +840,9 @@
         <v>5.73</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
-      <c r="A12" t="s">
-        <v>11</v>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B12">
         <v>0</v>

</xml_diff>